<commit_message>
feat: exercício 4  - feito
</commit_message>
<xml_diff>
--- a/modulos/03-Back-end/secao3_Funcoes_SQL_JOINs_e_Normalizacao/Dia3-Transformando_ideias_em_um_modelo_de_banco_de_dados/exercicios.dia.3/Exercicios-normalizacao/03-exercicio_segunda-forma-normal_resposta.xlsx
+++ b/modulos/03-Back-end/secao3_Funcoes_SQL_JOINs_e_Normalizacao/Dia3-Transformando_ideias_em_um_modelo_de_banco_de_dados/exercicios.dia.3/Exercicios-normalizacao/03-exercicio_segunda-forma-normal_resposta.xlsx
@@ -110,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -164,12 +164,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -313,7 +307,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -395,14 +389,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -486,7 +472,7 @@
   <dimension ref="F1:L27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -753,7 +739,7 @@
       <c r="F18" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="20" t="s">
         <v>12</v>
       </c>
       <c r="H18" s="20" t="n">
@@ -768,7 +754,7 @@
       <c r="F19" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="19" t="s">
         <v>8</v>
       </c>
       <c r="H19" s="19" t="n">

</xml_diff>